<commit_message>
Just a small edit of excel file.
</commit_message>
<xml_diff>
--- a/ukol_3/latex/statistics.xlsx
+++ b/ukol_3/latex/statistics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>N. of generated boards: 10,000</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -294,8 +297,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="466257664"/>
-        <c:axId val="466258840"/>
+        <c:axId val="298895960"/>
+        <c:axId val="143290456"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -404,7 +407,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="466257664"/>
+        <c:axId val="298895960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,7 +511,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466258840"/>
+        <c:crossAx val="143290456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -516,7 +519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="466258840"/>
+        <c:axId val="143290456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -633,7 +636,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466257664"/>
+        <c:crossAx val="298895960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1523,9 +1526,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M29"/>
+  <dimension ref="A2:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="V44" sqref="V44"/>
     </sheetView>
   </sheetViews>
@@ -1859,6 +1862,11 @@
         <v>0.93859999999999999</v>
       </c>
     </row>
+    <row r="44" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V44" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>